<commit_message>
updated 'original' band tags
</commit_message>
<xml_diff>
--- a/data/cholt_data.xlsx
+++ b/data/cholt_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Personal Folders\Dickerson\cholt\dash\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147937E1-678C-430E-AFA1-B157E56196BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7373AF01-BFDD-48AF-AB37-94AF379733F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12983" uniqueCount="3194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12984" uniqueCount="3195">
   <si>
     <t>Name</t>
   </si>
@@ -9614,6 +9614,9 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
@@ -42490,7 +42493,7 @@
   <dimension ref="A1:H388"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42637,7 +42640,7 @@
         <v>669</v>
       </c>
       <c r="C17" t="s">
-        <v>3112</v>
+        <v>3194</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -42646,6 +42649,9 @@
       <c r="A18" t="s">
         <v>876</v>
       </c>
+      <c r="C18" t="s">
+        <v>3194</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
@@ -42920,7 +42926,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>3112</v>
+        <v>3194</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -43980,7 +43986,7 @@
         <v>667</v>
       </c>
       <c r="C208" t="s">
-        <v>3112</v>
+        <v>3194</v>
       </c>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
@@ -44886,7 +44892,7 @@
         <v>619</v>
       </c>
       <c r="C337" t="s">
-        <v>3112</v>
+        <v>3194</v>
       </c>
       <c r="D337" s="3"/>
       <c r="E337" s="3"/>
@@ -45155,7 +45161,7 @@
         <v>668</v>
       </c>
       <c r="C375" t="s">
-        <v>3112</v>
+        <v>3194</v>
       </c>
       <c r="D375" s="3"/>
       <c r="E375" s="3"/>

</xml_diff>

<commit_message>
added more data points to bands
</commit_message>
<xml_diff>
--- a/data/cholt_data.xlsx
+++ b/data/cholt_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Personal Folders\Dickerson\cholt\dash\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7373AF01-BFDD-48AF-AB37-94AF379733F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4F5F69-FE2E-47CA-9550-C6F8658A383B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12984" uniqueCount="3195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13053" uniqueCount="3204">
   <si>
     <t>Name</t>
   </si>
@@ -9617,6 +9617,33 @@
   </si>
   <si>
     <t>Original</t>
+  </si>
+  <si>
+    <t>KISS</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Local DFW</t>
+  </si>
+  <si>
+    <t>CSNY</t>
+  </si>
+  <si>
+    <t>Floyd</t>
+  </si>
+  <si>
+    <t>Beach Boys</t>
+  </si>
+  <si>
+    <t>Simon and Garfunkel</t>
+  </si>
+  <si>
+    <t>Loal DFW</t>
+  </si>
+  <si>
+    <t>Hamilton OST</t>
   </si>
 </sst>
 </file>
@@ -42493,7 +42520,7 @@
   <dimension ref="A1:H388"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42534,7 +42561,9 @@
       <c r="A2" t="s">
         <v>859</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>609</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -42562,7 +42591,9 @@
       <c r="A6" t="s">
         <v>614</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>3195</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -42583,7 +42614,9 @@
       <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -42625,7 +42658,9 @@
       <c r="A15" t="s">
         <v>586</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -42642,7 +42677,9 @@
       <c r="C17" t="s">
         <v>3194</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -42652,7 +42689,9 @@
       <c r="C18" t="s">
         <v>3194</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -42666,14 +42705,18 @@
       <c r="A20" t="s">
         <v>201</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>662</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -42708,7 +42751,9 @@
       <c r="A26" t="s">
         <v>740</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>690</v>
+      </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -42750,14 +42795,18 @@
       <c r="A32" t="s">
         <v>646</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>728</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -42890,14 +42939,18 @@
       <c r="A52" t="s">
         <v>605</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="3" t="s">
+        <v>605</v>
+      </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>791</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>605</v>
+      </c>
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -42928,14 +42981,21 @@
       <c r="C57" t="s">
         <v>3194</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>666</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="C58" t="s">
+        <v>3194</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -42963,14 +43023,18 @@
       <c r="A62" t="s">
         <v>623</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>647</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -43040,7 +43104,9 @@
       <c r="A73" t="s">
         <v>142</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>3199</v>
+      </c>
       <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -43075,7 +43141,9 @@
       <c r="A78" t="s">
         <v>498</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="3" t="s">
+        <v>3200</v>
+      </c>
       <c r="E78" s="3"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -43194,14 +43262,18 @@
       <c r="A95" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="E95" s="3"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>651</v>
       </c>
-      <c r="D96" s="3"/>
+      <c r="D96" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="E96" s="3"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -43257,7 +43329,9 @@
       <c r="A104" t="s">
         <v>599</v>
       </c>
-      <c r="D104" s="3"/>
+      <c r="D104" s="3" t="s">
+        <v>599</v>
+      </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -43334,14 +43408,18 @@
       <c r="A115" t="s">
         <v>685</v>
       </c>
-      <c r="D115" s="3"/>
+      <c r="D115" s="3" t="s">
+        <v>685</v>
+      </c>
       <c r="E115" s="3"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>43</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E116" s="3"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -43362,7 +43440,9 @@
       <c r="A119" t="s">
         <v>148</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="E119" s="3"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -43453,14 +43533,18 @@
       <c r="A132" t="s">
         <v>802</v>
       </c>
-      <c r="D132" s="3"/>
+      <c r="D132" s="3" t="s">
+        <v>3203</v>
+      </c>
       <c r="E132" s="3"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>796</v>
       </c>
-      <c r="D133" s="3"/>
+      <c r="D133" s="3" t="s">
+        <v>3203</v>
+      </c>
       <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -43600,7 +43684,9 @@
       <c r="A153" t="s">
         <v>722</v>
       </c>
-      <c r="D153" s="3"/>
+      <c r="D153" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E153" s="3"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -43614,7 +43700,9 @@
       <c r="A155" t="s">
         <v>16</v>
       </c>
-      <c r="D155" s="3"/>
+      <c r="D155" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E155" s="3"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -43747,7 +43835,9 @@
       <c r="A174" t="s">
         <v>798</v>
       </c>
-      <c r="D174" s="3"/>
+      <c r="D174" s="3" t="s">
+        <v>599</v>
+      </c>
       <c r="E174" s="3"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -43922,14 +44012,18 @@
       <c r="A199" t="s">
         <v>134</v>
       </c>
-      <c r="D199" s="3"/>
+      <c r="D199" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="E199" s="3"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>705</v>
       </c>
-      <c r="D200" s="3"/>
+      <c r="D200" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="E200" s="3"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -43988,7 +44082,9 @@
       <c r="C208" t="s">
         <v>3194</v>
       </c>
-      <c r="D208" s="3"/>
+      <c r="D208" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E208" s="3"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -44002,28 +44098,36 @@
       <c r="A210" t="s">
         <v>581</v>
       </c>
-      <c r="D210" s="3"/>
+      <c r="D210" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E210" s="3"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>19</v>
       </c>
-      <c r="D211" s="3"/>
+      <c r="D211" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E211" s="3"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>622</v>
       </c>
-      <c r="D212" s="3"/>
+      <c r="D212" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E212" s="3"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>44</v>
       </c>
-      <c r="D213" s="3"/>
+      <c r="D213" s="3" t="s">
+        <v>3201</v>
+      </c>
       <c r="E213" s="3"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -44044,14 +44148,18 @@
       <c r="A216" t="s">
         <v>214</v>
       </c>
-      <c r="D216" s="3"/>
+      <c r="D216" s="3" t="s">
+        <v>671</v>
+      </c>
       <c r="E216" s="3"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>123</v>
       </c>
-      <c r="D217" s="3"/>
+      <c r="D217" s="3" t="s">
+        <v>685</v>
+      </c>
       <c r="E217" s="3"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -44065,7 +44173,9 @@
       <c r="A219" t="s">
         <v>246</v>
       </c>
-      <c r="D219" s="3"/>
+      <c r="D219" s="3" t="s">
+        <v>685</v>
+      </c>
       <c r="E219" s="3"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -44079,7 +44189,9 @@
       <c r="A221" t="s">
         <v>639</v>
       </c>
-      <c r="D221" s="3"/>
+      <c r="D221" s="3" t="s">
+        <v>3199</v>
+      </c>
       <c r="E221" s="3"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -44093,21 +44205,27 @@
       <c r="A223" t="s">
         <v>723</v>
       </c>
-      <c r="D223" s="3"/>
+      <c r="D223" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E223" s="3"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>587</v>
       </c>
-      <c r="D224" s="3"/>
+      <c r="D224" s="3" t="s">
+        <v>587</v>
+      </c>
       <c r="E224" s="3"/>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>768</v>
       </c>
-      <c r="D225" s="3"/>
+      <c r="D225" s="3" t="s">
+        <v>587</v>
+      </c>
       <c r="E225" s="3"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -44177,7 +44295,9 @@
       <c r="A235" t="s">
         <v>677</v>
       </c>
-      <c r="D235" s="3"/>
+      <c r="D235" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E235" s="3"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -44219,7 +44339,9 @@
       <c r="A241" t="s">
         <v>856</v>
       </c>
-      <c r="D241" s="3"/>
+      <c r="D241" s="3" t="s">
+        <v>3202</v>
+      </c>
       <c r="E241" s="3"/>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -44240,7 +44362,9 @@
       <c r="A244" t="s">
         <v>589</v>
       </c>
-      <c r="D244" s="3"/>
+      <c r="D244" s="3" t="s">
+        <v>3201</v>
+      </c>
       <c r="E244" s="3"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -44282,7 +44406,9 @@
       <c r="A250" t="s">
         <v>719</v>
       </c>
-      <c r="D250" s="3"/>
+      <c r="D250" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E250" s="3"/>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -44310,7 +44436,9 @@
       <c r="A254" t="s">
         <v>782</v>
       </c>
-      <c r="D254" s="3"/>
+      <c r="D254" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E254" s="3"/>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -44359,7 +44487,9 @@
       <c r="A261" t="s">
         <v>848</v>
       </c>
-      <c r="D261" s="3"/>
+      <c r="D261" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="E261" s="3"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -44373,7 +44503,9 @@
       <c r="A263" t="s">
         <v>107</v>
       </c>
-      <c r="D263" s="3"/>
+      <c r="D263" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="E263" s="3"/>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -44534,14 +44666,18 @@
       <c r="A286" t="s">
         <v>715</v>
       </c>
-      <c r="D286" s="3"/>
+      <c r="D286" s="3" t="s">
+        <v>3200</v>
+      </c>
       <c r="E286" s="3"/>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>588</v>
       </c>
-      <c r="D287" s="3"/>
+      <c r="D287" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E287" s="3"/>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -44856,7 +44992,9 @@
       <c r="A332" t="s">
         <v>877</v>
       </c>
-      <c r="D332" s="3"/>
+      <c r="D332" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E332" s="3"/>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -44894,7 +45032,9 @@
       <c r="C337" t="s">
         <v>3194</v>
       </c>
-      <c r="D337" s="3"/>
+      <c r="D337" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E337" s="3"/>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -44922,7 +45062,9 @@
       <c r="A341" t="s">
         <v>801</v>
       </c>
-      <c r="D341" s="3"/>
+      <c r="D341" s="3" t="s">
+        <v>3198</v>
+      </c>
       <c r="E341" s="3"/>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
@@ -44985,7 +45127,9 @@
       <c r="A350" t="s">
         <v>671</v>
       </c>
-      <c r="D350" s="3"/>
+      <c r="D350" s="3" t="s">
+        <v>671</v>
+      </c>
       <c r="E350" s="3"/>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -45013,7 +45157,12 @@
       <c r="A354" t="s">
         <v>854</v>
       </c>
-      <c r="D354" s="3"/>
+      <c r="C354" t="s">
+        <v>3194</v>
+      </c>
+      <c r="D354" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E354" s="3"/>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -45034,7 +45183,9 @@
       <c r="A357" t="s">
         <v>644</v>
       </c>
-      <c r="D357" s="3"/>
+      <c r="D357" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="E357" s="3"/>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -45048,14 +45199,18 @@
       <c r="A359" t="s">
         <v>278</v>
       </c>
-      <c r="D359" s="3"/>
+      <c r="D359" s="3" t="s">
+        <v>278</v>
+      </c>
       <c r="E359" s="3"/>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>697</v>
       </c>
-      <c r="D360" s="3"/>
+      <c r="D360" s="3" t="s">
+        <v>278</v>
+      </c>
       <c r="E360" s="3"/>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -45163,7 +45318,9 @@
       <c r="C375" t="s">
         <v>3194</v>
       </c>
-      <c r="D375" s="3"/>
+      <c r="D375" s="3" t="s">
+        <v>3197</v>
+      </c>
       <c r="E375" s="3"/>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
@@ -45198,7 +45355,9 @@
       <c r="A380" t="s">
         <v>690</v>
       </c>
-      <c r="D380" s="3"/>
+      <c r="D380" s="3" t="s">
+        <v>690</v>
+      </c>
       <c r="E380" s="3"/>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
@@ -45212,7 +45371,9 @@
       <c r="A382" t="s">
         <v>878</v>
       </c>
-      <c r="D382" s="3"/>
+      <c r="D382" s="3" t="s">
+        <v>3196</v>
+      </c>
       <c r="E382" s="3"/>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -45226,21 +45387,27 @@
       <c r="A384" t="s">
         <v>695</v>
       </c>
-      <c r="D384" s="3"/>
+      <c r="D384" s="3" t="s">
+        <v>695</v>
+      </c>
       <c r="E384" s="3"/>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>711</v>
       </c>
-      <c r="D385" s="3"/>
+      <c r="D385" s="3" t="s">
+        <v>695</v>
+      </c>
       <c r="E385" s="3"/>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>716</v>
       </c>
-      <c r="D386" s="3"/>
+      <c r="D386" s="3" t="s">
+        <v>695</v>
+      </c>
       <c r="E386" s="3"/>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>